<commit_message>
introduce spring boot admin
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzociaralli/work/bitbucket/test_env/dapr/dapr-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C64D2E-28E1-314E-9906-792C64900219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D6666E-53EE-8C4E-A7CF-4DB7EAA61A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="8120" windowWidth="34280" windowHeight="13020" xr2:uid="{585D81C7-7439-734E-8AC6-B66EDA43CEA6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>env</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>http_test_case_1</t>
+  </si>
+  <si>
+    <t>/callbackNoDapr</t>
   </si>
 </sst>
 </file>
@@ -203,8 +206,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C79F5FF-F344-214D-A5BA-0FA1DCA268BD}" name="Table1" displayName="Table1" ref="A1:O9" totalsRowShown="0">
-  <autoFilter ref="A1:O9" xr:uid="{8C79F5FF-F344-214D-A5BA-0FA1DCA268BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C79F5FF-F344-214D-A5BA-0FA1DCA268BD}" name="Table1" displayName="Table1" ref="A1:O13" totalsRowShown="0">
+  <autoFilter ref="A1:O13" xr:uid="{8C79F5FF-F344-214D-A5BA-0FA1DCA268BD}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{0AFF5BF5-E076-A74E-BE36-429B09843DFC}" name="env"/>
     <tableColumn id="11" xr3:uid="{025D51DF-1018-594E-8415-C451B8FA5F8D}" name="A instances"/>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00CEEFF2-1A17-174B-A7FA-13FB9E604E74}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,7 +557,7 @@
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
@@ -646,12 +649,14 @@
         <v>1</v>
       </c>
       <c r="M2" s="2">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N2" s="2">
         <v>0</v>
       </c>
-      <c r="O2" s="1"/>
+      <c r="O2" s="1">
+        <v>922.1</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -732,19 +737,19 @@
         <v>9</v>
       </c>
       <c r="K4" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2">
-        <v>418</v>
+        <v>310</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>2265.8000000000002</v>
+        <v>2324.6999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -967,19 +972,187 @@
         <v>16</v>
       </c>
       <c r="K9" s="2">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="L9" s="2">
         <v>1</v>
       </c>
       <c r="M9" s="2">
-        <v>1256</v>
+        <v>1657</v>
       </c>
       <c r="N9" s="2">
         <v>0</v>
       </c>
       <c r="O9" s="1">
-        <v>2351.1999999999998</v>
+        <v>2604.1999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2">
+        <v>10</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>19</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="1">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="2">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>127</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="1">
+        <v>2280.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I12" s="2">
+        <v>100</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="2">
+        <v>25</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>159</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="1">
+        <v>2924.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I13" s="2">
+        <v>250</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2">
+        <v>84</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>517</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="1">
+        <v>2722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>